<commit_message>
Day_8 | DA 19
</commit_message>
<xml_diff>
--- a/Batch/19/Day_8_Date_functions.xlsx
+++ b/Batch/19/Day_8_Date_functions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29024"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Work\Acciojob\Modules\Excel\Batch\18\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Work\Acciojob\Modules\Excel\Batch\19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466FBC86-2687-400B-A29D-71E5E226A329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4455F99D-7673-4680-896C-2B3078572A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5409,7 +5409,7 @@
       </c>
       <c r="C7" s="20">
         <f ca="1">NOW() +B3</f>
-        <v>45805.91914189815</v>
+        <v>45847.897718981483</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>32</v>

</xml_diff>